<commit_message>
Added the two types of files: one for +/-1 approach and one for carboneutrality. Did not separate sub-categories for carbon fossil/biogenic/land use in CC related impact categories.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei310/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei310/ei_iw_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82931717-F56C-42C3-83EF-564A994C9C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72EE1E2-8DD8-40C2-BF42-D4A3EB0A46E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4778" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4770" uniqueCount="1966">
   <si>
     <t>iw name</t>
   </si>
@@ -6290,9 +6290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12080,7 +12078,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="545" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>533</v>
       </c>
@@ -12091,7 +12089,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="546" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>980</v>
       </c>
@@ -12102,7 +12100,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="547" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>283</v>
       </c>
@@ -12113,7 +12111,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="548" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>284</v>
       </c>
@@ -12124,7 +12122,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="549" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>981</v>
       </c>
@@ -12132,7 +12130,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="550" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>982</v>
       </c>
@@ -12143,7 +12141,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="551" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>983</v>
       </c>
@@ -12154,7 +12152,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="552" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A552" t="s">
         <v>984</v>
       </c>
@@ -12165,7 +12163,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="553" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>285</v>
       </c>
@@ -12176,7 +12174,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="554" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>286</v>
       </c>
@@ -12187,7 +12185,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="555" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>287</v>
       </c>
@@ -12198,7 +12196,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="556" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>288</v>
       </c>
@@ -12209,7 +12207,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="557" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>289</v>
       </c>
@@ -12220,7 +12218,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="558" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>559</v>
       </c>
@@ -12231,35 +12229,23 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="559" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>985</v>
       </c>
-      <c r="B559" t="s">
-        <v>556</v>
-      </c>
       <c r="C559" t="s">
         <v>1578</v>
       </c>
-      <c r="D559" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="560" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>986</v>
       </c>
-      <c r="B560" t="s">
-        <v>557</v>
-      </c>
       <c r="C560" t="s">
         <v>1578</v>
       </c>
-      <c r="D560" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="561" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>560</v>
       </c>
@@ -12270,7 +12256,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="562" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
         <v>547</v>
       </c>
@@ -12281,21 +12267,15 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="563" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>987</v>
       </c>
-      <c r="B563" t="s">
-        <v>560</v>
-      </c>
       <c r="C563" t="s">
         <v>1578</v>
       </c>
-      <c r="D563" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="564" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
         <v>988</v>
       </c>
@@ -12303,7 +12283,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="565" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
         <v>989</v>
       </c>
@@ -12311,7 +12291,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="566" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
         <v>990</v>
       </c>
@@ -12319,7 +12299,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="567" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>991</v>
       </c>
@@ -12327,7 +12307,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="568" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
         <v>992</v>
       </c>
@@ -12335,7 +12315,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="569" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
         <v>993</v>
       </c>
@@ -12343,7 +12323,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="570" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>994</v>
       </c>
@@ -12351,7 +12331,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="571" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>506</v>
       </c>
@@ -12362,7 +12342,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="572" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>995</v>
       </c>
@@ -12370,7 +12350,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="573" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>290</v>
       </c>
@@ -12381,7 +12361,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="574" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>996</v>
       </c>
@@ -12389,7 +12369,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="575" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>291</v>
       </c>
@@ -12400,7 +12380,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="576" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>292</v>
       </c>
@@ -15295,7 +15275,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="849" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="849" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
         <v>360</v>
       </c>
@@ -15306,7 +15286,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="850" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="850" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
         <v>361</v>
       </c>
@@ -15317,7 +15297,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="851" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="851" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
         <v>362</v>
       </c>
@@ -15328,7 +15308,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="852" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="852" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
         <v>1150</v>
       </c>
@@ -15339,7 +15319,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="853" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="853" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
         <v>722</v>
       </c>
@@ -15350,7 +15330,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="854" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="854" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
         <v>363</v>
       </c>
@@ -15361,7 +15341,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="855" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="855" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
         <v>1151</v>
       </c>
@@ -15369,7 +15349,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="856" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="856" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
         <v>479</v>
       </c>
@@ -15380,7 +15360,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="857" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="857" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
         <v>1152</v>
       </c>
@@ -15388,21 +15368,15 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="858" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="858" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A858" t="s">
         <v>1153</v>
       </c>
-      <c r="B858" t="s">
-        <v>85</v>
-      </c>
       <c r="C858" t="s">
         <v>1578</v>
       </c>
-      <c r="D858" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="859" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
         <v>1154</v>
       </c>
@@ -15410,7 +15384,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="860" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="860" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A860" t="s">
         <v>1155</v>
       </c>
@@ -15418,7 +15392,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="861" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="861" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
         <v>1156</v>
       </c>
@@ -15426,7 +15400,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="862" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="862" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
         <v>1157</v>
       </c>
@@ -15434,7 +15408,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="863" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="863" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
         <v>365</v>
       </c>
@@ -15445,7 +15419,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="864" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="864" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
         <v>366</v>
       </c>
@@ -17672,7 +17646,7 @@
         <v>564</v>
       </c>
       <c r="B1078" t="s">
-        <v>564</v>
+        <v>47</v>
       </c>
       <c r="C1078" t="s">
         <v>1578</v>
@@ -20060,7 +20034,7 @@
         <v>472</v>
       </c>
       <c r="B1300" t="s">
-        <v>1965</v>
+        <v>472</v>
       </c>
       <c r="C1300" t="s">
         <v>1578</v>
@@ -24227,7 +24201,7 @@
         <v>1779</v>
       </c>
       <c r="B1708" t="s">
-        <v>472</v>
+        <v>1965</v>
       </c>
       <c r="C1708">
         <v>3.9</v>

</xml_diff>

<commit_message>
Final corrections for v2.1. Still need to update methodology files and report of changes.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei310/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei310/ei_iw_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72EE1E2-8DD8-40C2-BF42-D4A3EB0A46E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995A690B-DE5D-4EAF-A218-02A7079C8C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4770" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4768" uniqueCount="1966">
   <si>
     <t>iw name</t>
   </si>
@@ -5542,9 +5542,6 @@
     <t>Carbon dioxide, biogenic, release</t>
   </si>
   <si>
-    <t>Carbon monoxide, biogenic, release</t>
-  </si>
-  <si>
     <t>BOD</t>
   </si>
   <si>
@@ -5921,6 +5918,9 @@
   </si>
   <si>
     <t>Vanadium(V)</t>
+  </si>
+  <si>
+    <t>Carbon monoxide, biogenic</t>
   </si>
 </sst>
 </file>
@@ -6290,7 +6290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7204,7 +7206,7 @@
         <v>784</v>
       </c>
       <c r="B84" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C84" t="s">
         <v>1578</v>
@@ -7728,7 +7730,7 @@
         <v>482</v>
       </c>
       <c r="B133" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="C133" t="s">
         <v>1578</v>
@@ -8070,7 +8072,7 @@
         <v>811</v>
       </c>
       <c r="B166" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="C166" t="s">
         <v>1578</v>
@@ -8245,7 +8247,7 @@
         <v>820</v>
       </c>
       <c r="B183" t="s">
-        <v>1837</v>
+        <v>820</v>
       </c>
       <c r="C183" t="s">
         <v>1578</v>
@@ -8289,7 +8291,7 @@
         <v>822</v>
       </c>
       <c r="B187" t="s">
-        <v>1839</v>
+        <v>1965</v>
       </c>
       <c r="C187" t="s">
         <v>1578</v>
@@ -8770,7 +8772,7 @@
         <v>843</v>
       </c>
       <c r="B234" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="C234" t="s">
         <v>1578</v>
@@ -8784,7 +8786,7 @@
         <v>155</v>
       </c>
       <c r="B235" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="C235" t="s">
         <v>1578</v>
@@ -8817,7 +8819,7 @@
         <v>707</v>
       </c>
       <c r="B238" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="C238" t="s">
         <v>1578</v>
@@ -9072,7 +9074,7 @@
         <v>483</v>
       </c>
       <c r="B262" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="C262" t="s">
         <v>1578</v>
@@ -9248,7 +9250,7 @@
         <v>873</v>
       </c>
       <c r="B278" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="C278" t="s">
         <v>1578</v>
@@ -12650,7 +12652,7 @@
         <v>717</v>
       </c>
       <c r="B602" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="C602" t="s">
         <v>1578</v>
@@ -14335,7 +14337,7 @@
         <v>1078</v>
       </c>
       <c r="B762" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="C762" t="s">
         <v>1578</v>
@@ -14995,7 +14997,7 @@
         <v>1126</v>
       </c>
       <c r="B822" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
       <c r="C822" t="s">
         <v>1578</v>
@@ -15006,7 +15008,7 @@
         <v>1127</v>
       </c>
       <c r="B823" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
       <c r="C823" t="s">
         <v>1578</v>
@@ -15028,7 +15030,7 @@
         <v>1129</v>
       </c>
       <c r="B825" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
       <c r="C825" t="s">
         <v>1578</v>
@@ -15159,9 +15161,6 @@
       <c r="A837" t="s">
         <v>1141</v>
       </c>
-      <c r="B837" t="s">
-        <v>1574</v>
-      </c>
       <c r="C837" t="s">
         <v>1578</v>
       </c>
@@ -15170,9 +15169,6 @@
       <c r="A838" t="s">
         <v>1142</v>
       </c>
-      <c r="B838" t="s">
-        <v>1574</v>
-      </c>
       <c r="C838" t="s">
         <v>1578</v>
       </c>
@@ -17213,7 +17209,7 @@
         <v>1238</v>
       </c>
       <c r="B1034" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="C1034" t="s">
         <v>1578</v>
@@ -18205,7 +18201,7 @@
         <v>1287</v>
       </c>
       <c r="B1131" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="C1131" t="s">
         <v>1578</v>
@@ -20045,7 +20041,7 @@
         <v>1430</v>
       </c>
       <c r="B1301" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C1301" t="s">
         <v>1578</v>
@@ -20412,7 +20408,7 @@
         <v>1455</v>
       </c>
       <c r="B1339" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="C1339" t="s">
         <v>1578</v>
@@ -21547,7 +21543,7 @@
     </row>
     <row r="1452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1452" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="C1452">
         <v>3.9</v>
@@ -21569,7 +21565,7 @@
         <v>1602</v>
       </c>
       <c r="B1454" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="C1454">
         <v>3.9</v>
@@ -21624,7 +21620,7 @@
         <v>1606</v>
       </c>
       <c r="B1459" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="C1459">
         <v>3.9</v>
@@ -21643,7 +21639,7 @@
         <v>1607</v>
       </c>
       <c r="B1461" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C1461">
         <v>3.9</v>
@@ -21651,7 +21647,7 @@
     </row>
     <row r="1462" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1462" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="C1462">
         <v>3.9</v>
@@ -21673,7 +21669,7 @@
         <v>1609</v>
       </c>
       <c r="B1464" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="C1464">
         <v>3.9</v>
@@ -21695,7 +21691,7 @@
         <v>1610</v>
       </c>
       <c r="B1466" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="C1466">
         <v>3.9</v>
@@ -21703,7 +21699,7 @@
     </row>
     <row r="1467" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1467" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="C1467">
         <v>3.9</v>
@@ -21711,7 +21707,7 @@
     </row>
     <row r="1468" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1468" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="C1468">
         <v>3.9</v>
@@ -21719,10 +21715,10 @@
     </row>
     <row r="1469" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1469" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B1469" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="C1469">
         <v>3.9</v>
@@ -21752,7 +21748,7 @@
         <v>1612</v>
       </c>
       <c r="B1472" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="C1472">
         <v>3.9</v>
@@ -21861,7 +21857,7 @@
         <v>589</v>
       </c>
       <c r="B1483" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="C1483">
         <v>3.9</v>
@@ -21949,7 +21945,7 @@
         <v>1624</v>
       </c>
       <c r="B1491" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="C1491">
         <v>3.9</v>
@@ -21982,7 +21978,7 @@
         <v>1626</v>
       </c>
       <c r="B1494" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="C1494">
         <v>3.9</v>
@@ -22160,7 +22156,7 @@
     </row>
     <row r="1511" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1511" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="C1511">
         <v>3.9</v>
@@ -22288,10 +22284,10 @@
     </row>
     <row r="1524" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1524" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B1524" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="C1524">
         <v>3.9</v>
@@ -22354,10 +22350,10 @@
     </row>
     <row r="1530" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1530" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B1530" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="C1530">
         <v>3.9</v>
@@ -22684,7 +22680,7 @@
     </row>
     <row r="1560" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1560" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="C1560">
         <v>3.9</v>
@@ -22703,7 +22699,7 @@
     </row>
     <row r="1562" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1562" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B1562" t="s">
         <v>533</v>
@@ -22714,7 +22710,7 @@
     </row>
     <row r="1563" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1563" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B1563" t="s">
         <v>533</v>
@@ -22777,7 +22773,7 @@
         <v>1682</v>
       </c>
       <c r="B1569" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="C1569">
         <v>3.9</v>
@@ -22851,7 +22847,7 @@
     </row>
     <row r="1576" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1576" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="C1576">
         <v>3.9</v>
@@ -22881,7 +22877,7 @@
         <v>1689</v>
       </c>
       <c r="B1579" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="C1579">
         <v>3.9</v>
@@ -22977,7 +22973,7 @@
         <v>1697</v>
       </c>
       <c r="B1588" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="C1588">
         <v>3.9</v>
@@ -22999,7 +22995,7 @@
         <v>1699</v>
       </c>
       <c r="B1590" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="C1590">
         <v>3.9</v>
@@ -23010,7 +23006,7 @@
         <v>1700</v>
       </c>
       <c r="B1591" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="C1591">
         <v>3.9</v>
@@ -23095,7 +23091,7 @@
     </row>
     <row r="1599" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1599" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C1599">
         <v>3.9</v>
@@ -23103,7 +23099,7 @@
     </row>
     <row r="1600" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1600" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="C1600">
         <v>3.9</v>
@@ -23158,7 +23154,7 @@
         <v>1712</v>
       </c>
       <c r="B1605" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="C1605">
         <v>3.9</v>
@@ -23259,7 +23255,7 @@
     </row>
     <row r="1615" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1615" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="C1615">
         <v>3.9</v>
@@ -23335,7 +23331,7 @@
     </row>
     <row r="1623" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1623" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="C1623">
         <v>3.9</v>
@@ -23387,7 +23383,7 @@
     </row>
     <row r="1628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1628" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="C1628">
         <v>3.9</v>
@@ -23395,7 +23391,7 @@
     </row>
     <row r="1629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1629" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="C1629">
         <v>3.9</v>
@@ -23436,7 +23432,7 @@
     </row>
     <row r="1633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1633" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="C1633">
         <v>3.9</v>
@@ -23529,7 +23525,7 @@
     </row>
     <row r="1642" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1642" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="C1642">
         <v>3.9</v>
@@ -23575,7 +23571,7 @@
     </row>
     <row r="1647" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1647" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="C1647">
         <v>3.9</v>
@@ -23635,7 +23631,7 @@
         <v>1742</v>
       </c>
       <c r="B1653" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="C1653">
         <v>3.9</v>
@@ -23657,7 +23653,7 @@
         <v>1743</v>
       </c>
       <c r="B1655" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="C1655">
         <v>3.9</v>
@@ -23819,7 +23815,7 @@
     </row>
     <row r="1670" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1670" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="C1670">
         <v>3.9</v>
@@ -23849,7 +23845,7 @@
     </row>
     <row r="1673" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1673" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="C1673">
         <v>3.9</v>
@@ -23857,10 +23853,10 @@
     </row>
     <row r="1674" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1674" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B1674" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="C1674">
         <v>3.9</v>
@@ -23868,7 +23864,7 @@
     </row>
     <row r="1675" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1675" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="C1675">
         <v>3.9</v>
@@ -23876,10 +23872,10 @@
     </row>
     <row r="1676" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1676" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B1676" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="C1676">
         <v>3.9</v>
@@ -23887,10 +23883,10 @@
     </row>
     <row r="1677" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1677" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B1677" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="C1677">
         <v>3.9</v>
@@ -23939,7 +23935,7 @@
     </row>
     <row r="1682" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1682" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="C1682">
         <v>3.9</v>
@@ -24073,7 +24069,7 @@
         <v>1769</v>
       </c>
       <c r="B1695" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="C1695">
         <v>3.9</v>
@@ -24081,10 +24077,10 @@
     </row>
     <row r="1696" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1696" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B1696" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="C1696">
         <v>3.9</v>
@@ -24114,7 +24110,7 @@
         <v>1775</v>
       </c>
       <c r="B1699" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="C1699">
         <v>3.9</v>
@@ -24165,10 +24161,10 @@
     </row>
     <row r="1705" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1705" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B1705" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="C1705">
         <v>3.9</v>
@@ -24176,10 +24172,10 @@
     </row>
     <row r="1706" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1706" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B1706" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="C1706">
         <v>3.9</v>
@@ -24201,7 +24197,7 @@
         <v>1779</v>
       </c>
       <c r="B1708" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C1708">
         <v>3.9</v>
@@ -24236,7 +24232,7 @@
     </row>
     <row r="1712" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1712" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="C1712">
         <v>3.9</v>
@@ -24266,7 +24262,7 @@
         <v>1782</v>
       </c>
       <c r="B1715" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="C1715">
         <v>3.9</v>
@@ -24329,7 +24325,7 @@
     </row>
     <row r="1721" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1721" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B1721" t="s">
         <v>7</v>
@@ -24340,7 +24336,7 @@
     </row>
     <row r="1722" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1722" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="B1722" t="s">
         <v>8</v>
@@ -24351,7 +24347,7 @@
     </row>
     <row r="1723" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1723" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="B1723" t="s">
         <v>9</v>
@@ -24362,7 +24358,7 @@
     </row>
     <row r="1724" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1724" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B1724" t="s">
         <v>10</v>
@@ -24373,7 +24369,7 @@
     </row>
     <row r="1725" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1725" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B1725" t="s">
         <v>227</v>
@@ -24384,7 +24380,7 @@
     </row>
     <row r="1726" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1726" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B1726" t="s">
         <v>11</v>
@@ -24395,7 +24391,7 @@
     </row>
     <row r="1727" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1727" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B1727" t="s">
         <v>12</v>
@@ -24406,7 +24402,7 @@
     </row>
     <row r="1728" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1728" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B1728" t="s">
         <v>14</v>
@@ -24428,7 +24424,7 @@
     </row>
     <row r="1730" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1730" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B1730" t="s">
         <v>15</v>
@@ -24450,7 +24446,7 @@
     </row>
     <row r="1732" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1732" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B1732" t="s">
         <v>16</v>
@@ -24472,7 +24468,7 @@
     </row>
     <row r="1734" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1734" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B1734" t="s">
         <v>604</v>
@@ -24483,7 +24479,7 @@
     </row>
     <row r="1735" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1735" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B1735" t="s">
         <v>17</v>
@@ -24527,7 +24523,7 @@
     </row>
     <row r="1739" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1739" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B1739" t="s">
         <v>558</v>
@@ -24538,7 +24534,7 @@
     </row>
     <row r="1740" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1740" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="C1740" t="s">
         <v>1798</v>
@@ -24546,7 +24542,7 @@
     </row>
     <row r="1741" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1741" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="C1741" t="s">
         <v>1798</v>
@@ -24554,7 +24550,7 @@
     </row>
     <row r="1742" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1742" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="C1742" t="s">
         <v>1798</v>
@@ -24562,7 +24558,7 @@
     </row>
     <row r="1743" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1743" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B1743" t="s">
         <v>379</v>
@@ -24573,10 +24569,10 @@
     </row>
     <row r="1744" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1744" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B1744" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="C1744" t="s">
         <v>1798</v>
@@ -24584,7 +24580,7 @@
     </row>
     <row r="1745" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1745" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B1745" t="s">
         <v>571</v>
@@ -24595,7 +24591,7 @@
     </row>
     <row r="1746" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1746" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B1746" t="s">
         <v>24</v>
@@ -24606,7 +24602,7 @@
     </row>
     <row r="1747" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1747" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B1747" t="s">
         <v>614</v>
@@ -24628,7 +24624,7 @@
     </row>
     <row r="1749" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1749" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B1749" t="s">
         <v>25</v>
@@ -24650,7 +24646,7 @@
     </row>
     <row r="1751" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1751" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B1751" t="s">
         <v>380</v>
@@ -24661,7 +24657,7 @@
     </row>
     <row r="1752" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1752" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="B1752" t="s">
         <v>27</v>
@@ -24672,7 +24668,7 @@
     </row>
     <row r="1753" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1753" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B1753" t="s">
         <v>28</v>
@@ -24694,7 +24690,7 @@
     </row>
     <row r="1755" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1755" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B1755" t="s">
         <v>29</v>
@@ -24705,7 +24701,7 @@
     </row>
     <row r="1756" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1756" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="B1756" t="s">
         <v>204</v>
@@ -24716,7 +24712,7 @@
     </row>
     <row r="1757" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1757" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B1757" t="s">
         <v>381</v>
@@ -24727,10 +24723,10 @@
     </row>
     <row r="1758" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1758" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B1758" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="C1758" t="s">
         <v>1798</v>
@@ -24738,7 +24734,7 @@
     </row>
     <row r="1759" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1759" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B1759" t="s">
         <v>212</v>
@@ -24749,7 +24745,7 @@
     </row>
     <row r="1760" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1760" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="B1760" t="s">
         <v>106</v>
@@ -24760,7 +24756,7 @@
     </row>
     <row r="1761" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1761" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="B1761" t="s">
         <v>759</v>
@@ -24771,7 +24767,7 @@
     </row>
     <row r="1762" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1762" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B1762" t="s">
         <v>13</v>
@@ -24782,7 +24778,7 @@
     </row>
     <row r="1763" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1763" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B1763" t="s">
         <v>274</v>
@@ -24793,10 +24789,10 @@
     </row>
     <row r="1764" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1764" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B1764" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="C1764" t="s">
         <v>1798</v>
@@ -24804,7 +24800,7 @@
     </row>
     <row r="1765" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1765" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B1765" t="s">
         <v>107</v>
@@ -24815,7 +24811,7 @@
     </row>
     <row r="1766" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1766" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B1766" t="s">
         <v>228</v>
@@ -24826,7 +24822,7 @@
     </row>
     <row r="1767" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1767" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B1767" t="s">
         <v>19</v>
@@ -24859,7 +24855,7 @@
     </row>
     <row r="1770" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1770" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B1770" t="s">
         <v>587</v>
@@ -24870,7 +24866,7 @@
     </row>
     <row r="1771" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1771" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B1771" t="s">
         <v>54</v>
@@ -24881,7 +24877,7 @@
     </row>
     <row r="1772" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1772" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B1772" t="s">
         <v>643</v>
@@ -24892,7 +24888,7 @@
     </row>
     <row r="1773" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1773" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B1773" t="s">
         <v>56</v>
@@ -24919,7 +24915,7 @@
     </row>
     <row r="1776" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1776" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B1776" t="s">
         <v>31</v>
@@ -24952,7 +24948,7 @@
     </row>
     <row r="1779" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1779" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B1779" t="s">
         <v>105</v>
@@ -24963,7 +24959,7 @@
     </row>
     <row r="1780" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1780" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B1780" t="s">
         <v>18</v>
@@ -24985,7 +24981,7 @@
     </row>
     <row r="1782" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1782" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B1782" t="s">
         <v>577</v>
@@ -24996,7 +24992,7 @@
     </row>
     <row r="1783" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1783" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B1783" t="s">
         <v>610</v>
@@ -25007,7 +25003,7 @@
     </row>
     <row r="1784" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1784" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B1784" t="s">
         <v>108</v>
@@ -25018,7 +25014,7 @@
     </row>
     <row r="1785" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1785" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B1785" t="s">
         <v>375</v>
@@ -25029,7 +25025,7 @@
     </row>
     <row r="1786" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1786" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B1786" t="s">
         <v>20</v>
@@ -25051,7 +25047,7 @@
     </row>
     <row r="1788" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1788" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B1788" t="s">
         <v>252</v>
@@ -25062,7 +25058,7 @@
     </row>
     <row r="1789" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1789" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="C1789" t="s">
         <v>1798</v>
@@ -25081,7 +25077,7 @@
     </row>
     <row r="1791" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1791" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="C1791" t="s">
         <v>1798</v>
@@ -25089,7 +25085,7 @@
     </row>
     <row r="1792" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1792" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B1792" t="s">
         <v>404</v>
@@ -25100,7 +25096,7 @@
     </row>
     <row r="1793" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1793" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B1793" t="s">
         <v>497</v>
@@ -25111,7 +25107,7 @@
     </row>
     <row r="1794" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1794" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B1794" t="s">
         <v>53</v>
@@ -25155,10 +25151,10 @@
     </row>
     <row r="1798" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1798" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B1798" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="C1798" t="s">
         <v>1798</v>
@@ -25174,7 +25170,7 @@
     </row>
     <row r="1800" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1800" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B1800" t="s">
         <v>481</v>
@@ -25207,7 +25203,7 @@
     </row>
     <row r="1803" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1803" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B1803" t="s">
         <v>572</v>
@@ -25226,7 +25222,7 @@
     </row>
     <row r="1805" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1805" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B1805" t="s">
         <v>32</v>
@@ -25237,10 +25233,10 @@
     </row>
     <row r="1806" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1806" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B1806" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="C1806" t="s">
         <v>1798</v>
@@ -25248,7 +25244,7 @@
     </row>
     <row r="1807" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1807" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B1807" t="s">
         <v>33</v>
@@ -25270,7 +25266,7 @@
     </row>
     <row r="1809" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1809" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B1809" t="s">
         <v>1828</v>
@@ -25281,7 +25277,7 @@
     </row>
     <row r="1810" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1810" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B1810" t="s">
         <v>506</v>
@@ -25292,7 +25288,7 @@
     </row>
     <row r="1811" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1811" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B1811" t="s">
         <v>495</v>
@@ -25303,7 +25299,7 @@
     </row>
     <row r="1812" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1812" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="C1812" t="s">
         <v>1798</v>

</xml_diff>

<commit_message>
Update documentation for water availability human health and water scarcity indicators.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei310/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei310/ei_iw_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995A690B-DE5D-4EAF-A218-02A7079C8C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D513585-AD69-4CB1-ACD8-3232804F55C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4768" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4770" uniqueCount="1966">
   <si>
     <t>iw name</t>
   </si>
@@ -6291,7 +6291,7 @@
   <dimension ref="A1:D1812"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15161,6 +15161,9 @@
       <c r="A837" t="s">
         <v>1141</v>
       </c>
+      <c r="B837" t="s">
+        <v>1574</v>
+      </c>
       <c r="C837" t="s">
         <v>1578</v>
       </c>
@@ -15169,6 +15172,9 @@
       <c r="A838" t="s">
         <v>1142</v>
       </c>
+      <c r="B838" t="s">
+        <v>1574</v>
+      </c>
       <c r="C838" t="s">
         <v>1578</v>
       </c>
@@ -18793,7 +18799,7 @@
         <v>1340</v>
       </c>
       <c r="B1187" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C1187" t="s">
         <v>1578</v>
@@ -18804,7 +18810,7 @@
         <v>1341</v>
       </c>
       <c r="B1188" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C1188" t="s">
         <v>1578</v>
@@ -18826,7 +18832,7 @@
         <v>1343</v>
       </c>
       <c r="B1190" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C1190" t="s">
         <v>1578</v>
@@ -19453,7 +19459,7 @@
         <v>1400</v>
       </c>
       <c r="B1247" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C1247" t="s">
         <v>1578</v>
@@ -19464,7 +19470,7 @@
         <v>1401</v>
       </c>
       <c r="B1248" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C1248" t="s">
         <v>1578</v>
@@ -19486,7 +19492,7 @@
         <v>1403</v>
       </c>
       <c r="B1250" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C1250" t="s">
         <v>1578</v>

</xml_diff>

<commit_message>
New CC damage Fate factor modeling.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei310/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei310/ei_iw_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D513585-AD69-4CB1-ACD8-3232804F55C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35407907-A4B2-4FB3-BF70-ADE632FD915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4770" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4771" uniqueCount="1967">
   <si>
     <t>iw name</t>
   </si>
@@ -5921,6 +5921,9 @@
   </si>
   <si>
     <t>Carbon monoxide, biogenic</t>
+  </si>
+  <si>
+    <t>Avermectin B1</t>
   </si>
 </sst>
 </file>
@@ -6290,8 +6293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6577,6 +6580,9 @@
       <c r="A25" t="s">
         <v>766</v>
       </c>
+      <c r="B25" t="s">
+        <v>1966</v>
+      </c>
       <c r="C25" t="s">
         <v>1578</v>
       </c>

</xml_diff>